<commit_message>
EPICP-1 changes in DPEs from Tracy and Ines
</commit_message>
<xml_diff>
--- a/analyst/Ines/rmonize/data_proc_elem/DPE_EPICP_INES.xlsx
+++ b/analyst/Ines/rmonize/data_proc_elem/DPE_EPICP_INES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\analyst\Ines\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{AE058C4F-A81E-45B4-A5BF-3E4B4CAA7C36}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBAB8E61-325F-4EAE-9C0E-521F47AE8179}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="119">
   <si>
     <t>index</t>
   </si>
@@ -370,84 +370,20 @@
     <t>hip_f4</t>
   </si>
   <si>
-    <r>
-      <t>age0;DAT_REKR;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>date</t>
-    </r>
-  </si>
-  <si>
     <t>gj*4.184</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>age0+((</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">date </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>DAT_REKR)/365.25)</t>
-    </r>
-  </si>
-  <si>
     <t>gj [kJ] calculated in kcal</t>
   </si>
   <si>
-    <t>difference of FUP4 and baseline in years and then add this to age0</t>
+    <t>age_anth_f4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -459,13 +395,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -497,13 +426,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -844,8 +772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -932,17 +860,17 @@
       <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>110</v>
       </c>
       <c r="G3" t="s">
         <v>85</v>
       </c>
       <c r="H3" t="s">
+        <v>116</v>
+      </c>
+      <c r="I3" t="s">
         <v>117</v>
-      </c>
-      <c r="I3" t="s">
-        <v>119</v>
       </c>
       <c r="J3" t="s">
         <v>83</v>
@@ -961,7 +889,7 @@
       <c r="D4" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>89</v>
       </c>
       <c r="G4" t="s">
@@ -987,7 +915,7 @@
       <c r="D5" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>90</v>
       </c>
       <c r="G5" t="s">
@@ -1013,13 +941,13 @@
       <c r="D6" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="2" t="s">
         <v>92</v>
       </c>
       <c r="G6" t="s">
         <v>85</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="2" t="s">
         <v>93</v>
       </c>
       <c r="J6" t="s">
@@ -1039,7 +967,7 @@
       <c r="D7" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="2" t="s">
         <v>91</v>
       </c>
       <c r="G7" t="s">
@@ -1091,7 +1019,7 @@
       <c r="D9" t="s">
         <v>13</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G9" t="s">
@@ -1117,7 +1045,7 @@
       <c r="D10" t="s">
         <v>13</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G10" t="s">
@@ -1169,7 +1097,7 @@
       <c r="D12" t="s">
         <v>13</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="2" t="s">
         <v>113</v>
       </c>
       <c r="G12" t="s">
@@ -1195,7 +1123,7 @@
       <c r="D13" t="s">
         <v>13</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="2" t="s">
         <v>114</v>
       </c>
       <c r="G13" t="s">
@@ -1352,22 +1280,19 @@
         <v>13</v>
       </c>
       <c r="F19" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G19" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="I19" t="s">
-        <v>120</v>
+        <v>82</v>
       </c>
       <c r="J19" t="s">
         <v>83</v>
       </c>
       <c r="K19" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.3">
@@ -1380,7 +1305,7 @@
       <c r="D20" t="s">
         <v>13</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" s="2" t="s">
         <v>94</v>
       </c>
       <c r="G20" t="s">
@@ -1406,7 +1331,7 @@
       <c r="D21" t="s">
         <v>13</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="2" t="s">
         <v>95</v>
       </c>
       <c r="G21" t="s">
@@ -1432,7 +1357,7 @@
       <c r="D22" t="s">
         <v>13</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F22" s="2" t="s">
         <v>96</v>
       </c>
       <c r="G22" t="s">
@@ -1458,7 +1383,7 @@
       <c r="D23" t="s">
         <v>13</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F23" s="2" t="s">
         <v>97</v>
       </c>
       <c r="G23" t="s">
@@ -1484,7 +1409,7 @@
       <c r="D24" t="s">
         <v>13</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F24" s="2" t="s">
         <v>98</v>
       </c>
       <c r="G24" t="s">
@@ -1510,7 +1435,7 @@
       <c r="D25" t="s">
         <v>13</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F25" s="2" t="s">
         <v>99</v>
       </c>
       <c r="G25" t="s">
@@ -1536,7 +1461,7 @@
       <c r="D26" t="s">
         <v>13</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="F26" s="2" t="s">
         <v>100</v>
       </c>
       <c r="G26" t="s">
@@ -1562,7 +1487,7 @@
       <c r="D27" t="s">
         <v>13</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="F27" s="2" t="s">
         <v>101</v>
       </c>
       <c r="G27" t="s">
@@ -1588,13 +1513,13 @@
       <c r="D28" t="s">
         <v>13</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="F28" s="2" t="s">
         <v>102</v>
       </c>
       <c r="G28" t="s">
         <v>85</v>
       </c>
-      <c r="H28" s="3" t="s">
+      <c r="H28" s="2" t="s">
         <v>103</v>
       </c>
       <c r="J28" t="s">
@@ -1666,7 +1591,7 @@
       <c r="D31" t="s">
         <v>13</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="F31" s="2" t="s">
         <v>104</v>
       </c>
       <c r="G31" t="s">
@@ -1692,7 +1617,7 @@
       <c r="D32" t="s">
         <v>13</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="F32" s="2" t="s">
         <v>105</v>
       </c>
       <c r="G32" t="s">
@@ -1718,7 +1643,7 @@
       <c r="D33" t="s">
         <v>13</v>
       </c>
-      <c r="F33" s="3" t="s">
+      <c r="F33" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G33" t="s">
@@ -1744,7 +1669,7 @@
       <c r="D34" t="s">
         <v>13</v>
       </c>
-      <c r="F34" s="3" t="s">
+      <c r="F34" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G34" t="s">
@@ -1770,7 +1695,7 @@
       <c r="D35" t="s">
         <v>13</v>
       </c>
-      <c r="F35" s="3" t="s">
+      <c r="F35" s="2" t="s">
         <v>106</v>
       </c>
       <c r="G35" t="s">
@@ -1796,13 +1721,13 @@
       <c r="D36" t="s">
         <v>13</v>
       </c>
-      <c r="F36" s="3" t="s">
+      <c r="F36" s="2" t="s">
         <v>108</v>
       </c>
       <c r="G36" t="s">
         <v>85</v>
       </c>
-      <c r="H36" s="3" t="s">
+      <c r="H36" s="2" t="s">
         <v>107</v>
       </c>
       <c r="J36" t="s">

</xml_diff>

<commit_message>
EPICP-5 addressing some issues revealed by rmonize output concerning ENERGY, INC_ISC_STR, INC_HAEMO_STR; BMI_FUP & TOBACCO_D input data likely needs to be corrected but rmonize is correct
</commit_message>
<xml_diff>
--- a/analyst/Ines/rmonize/data_proc_elem/DPE_EPICP_INES.xlsx
+++ b/analyst/Ines/rmonize/data_proc_elem/DPE_EPICP_INES.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\analyst\Ines\rmonize\data_proc_elem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\analyst\Ines\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{3618EEF5-7AD4-4FC1-9FBA-35C55DEB3C5B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4B2C00A-F88C-4A69-BB5A-62B049E64521}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -322,9 +322,6 @@
     <t>GJ</t>
   </si>
   <si>
-    <t>GJ*4.184</t>
-  </si>
-  <si>
     <t>GJ [kJ] calculated in kcal</t>
   </si>
   <si>
@@ -377,6 +374,9 @@
   </si>
   <si>
     <t>KD+KM</t>
+  </si>
+  <si>
+    <t>GJ/4.184</t>
   </si>
 </sst>
 </file>
@@ -773,23 +773,23 @@
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="67" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="42.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>11</v>
       </c>
@@ -850,7 +850,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -867,10 +867,10 @@
         <v>85</v>
       </c>
       <c r="H3" t="s">
+        <v>118</v>
+      </c>
+      <c r="I3" t="s">
         <v>100</v>
-      </c>
-      <c r="I3" t="s">
-        <v>101</v>
       </c>
       <c r="J3" t="s">
         <v>83</v>
@@ -879,7 +879,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>16</v>
       </c>
@@ -905,7 +905,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>18</v>
       </c>
@@ -931,7 +931,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>20</v>
       </c>
@@ -957,7 +957,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>22</v>
       </c>
@@ -983,7 +983,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>24</v>
       </c>
@@ -1009,7 +1009,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>26</v>
       </c>
@@ -1035,7 +1035,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>28</v>
       </c>
@@ -1061,7 +1061,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>30</v>
       </c>
@@ -1087,7 +1087,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>32</v>
       </c>
@@ -1098,7 +1098,7 @@
         <v>13</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G12" t="s">
         <v>82</v>
@@ -1113,7 +1113,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>34</v>
       </c>
@@ -1124,7 +1124,7 @@
         <v>13</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G13" t="s">
         <v>82</v>
@@ -1139,7 +1139,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>36</v>
       </c>
@@ -1165,7 +1165,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>38</v>
       </c>
@@ -1191,7 +1191,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>40</v>
       </c>
@@ -1217,7 +1217,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>42</v>
       </c>
@@ -1243,7 +1243,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>44</v>
       </c>
@@ -1269,7 +1269,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>46</v>
       </c>
@@ -1295,7 +1295,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>48</v>
       </c>
@@ -1306,7 +1306,7 @@
         <v>13</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G20" t="s">
         <v>82</v>
@@ -1321,7 +1321,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>50</v>
       </c>
@@ -1332,7 +1332,7 @@
         <v>13</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G21" t="s">
         <v>82</v>
@@ -1347,7 +1347,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>52</v>
       </c>
@@ -1358,7 +1358,7 @@
         <v>13</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G22" t="s">
         <v>82</v>
@@ -1373,7 +1373,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>54</v>
       </c>
@@ -1384,7 +1384,7 @@
         <v>13</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G23" t="s">
         <v>82</v>
@@ -1399,7 +1399,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>56</v>
       </c>
@@ -1410,7 +1410,7 @@
         <v>13</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G24" t="s">
         <v>82</v>
@@ -1425,7 +1425,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>58</v>
       </c>
@@ -1436,7 +1436,7 @@
         <v>13</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G25" t="s">
         <v>82</v>
@@ -1451,7 +1451,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>60</v>
       </c>
@@ -1462,7 +1462,7 @@
         <v>13</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G26" t="s">
         <v>82</v>
@@ -1477,7 +1477,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>62</v>
       </c>
@@ -1488,7 +1488,7 @@
         <v>13</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G27" t="s">
         <v>82</v>
@@ -1503,7 +1503,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>64</v>
       </c>
@@ -1514,13 +1514,13 @@
         <v>13</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G28" t="s">
         <v>85</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J28" t="s">
         <v>83</v>
@@ -1529,7 +1529,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>66</v>
       </c>
@@ -1555,7 +1555,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>68</v>
       </c>
@@ -1581,7 +1581,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>70</v>
       </c>
@@ -1592,7 +1592,7 @@
         <v>13</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G31" t="s">
         <v>82</v>
@@ -1607,7 +1607,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>72</v>
       </c>
@@ -1618,7 +1618,7 @@
         <v>13</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G32" t="s">
         <v>82</v>
@@ -1633,7 +1633,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>74</v>
       </c>
@@ -1659,7 +1659,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>76</v>
       </c>
@@ -1685,7 +1685,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>78</v>
       </c>
@@ -1696,7 +1696,7 @@
         <v>13</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G35" t="s">
         <v>82</v>
@@ -1711,7 +1711,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>80</v>
       </c>
@@ -1722,13 +1722,13 @@
         <v>13</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G36" t="s">
         <v>85</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J36" t="s">
         <v>83</v>

</xml_diff>

<commit_message>
fix: Sodium, LDL, HDL, CHOL, TG => unit conversions in DPE unclear: correct algorithm for age_cancer, needs clarification
</commit_message>
<xml_diff>
--- a/analyst/Ines/rmonize/data_proc_elem/DPE_EPICP_INES.xlsx
+++ b/analyst/Ines/rmonize/data_proc_elem/DPE_EPICP_INES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\analyst\Ines\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4B2C00A-F88C-4A69-BB5A-62B049E64521}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46CA17F2-AB5A-4B4C-9715-510BFD9D8A7F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="123">
   <si>
     <t>index</t>
   </si>
@@ -301,9 +301,6 @@
     <t>corr_chol;corr_hdl</t>
   </si>
   <si>
-    <t>corr_chol - corr_hdl</t>
-  </si>
-  <si>
     <t>bmi_f4</t>
   </si>
   <si>
@@ -377,6 +374,21 @@
   </si>
   <si>
     <t>GJ/4.184</t>
+  </si>
+  <si>
+    <t>corr_hdl/38.67</t>
+  </si>
+  <si>
+    <t>(corr_chol - corr_hdl)/38.67</t>
+  </si>
+  <si>
+    <t>corr_chol/38.67</t>
+  </si>
+  <si>
+    <t>MNA*1000</t>
+  </si>
+  <si>
+    <t>corr_trigly/88.57</t>
   </si>
 </sst>
 </file>
@@ -772,8 +784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="C13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -783,7 +795,7 @@
     <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="42.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.140625" customWidth="1"/>
     <col min="9" max="9" width="27.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="25.28515625" bestFit="1" customWidth="1"/>
@@ -835,7 +847,7 @@
         <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G2" t="s">
         <v>82</v>
@@ -861,16 +873,16 @@
         <v>13</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G3" t="s">
         <v>85</v>
       </c>
       <c r="H3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J3" t="s">
         <v>83</v>
@@ -893,16 +905,16 @@
         <v>89</v>
       </c>
       <c r="G4" t="s">
-        <v>82</v>
-      </c>
-      <c r="H4" t="s">
-        <v>82</v>
+        <v>85</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>122</v>
       </c>
       <c r="J4" t="s">
         <v>83</v>
       </c>
       <c r="K4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -919,16 +931,16 @@
         <v>90</v>
       </c>
       <c r="G5" t="s">
-        <v>82</v>
-      </c>
-      <c r="H5" t="s">
-        <v>82</v>
+        <v>85</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="J5" t="s">
         <v>83</v>
       </c>
       <c r="K5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -948,7 +960,7 @@
         <v>85</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="J6" t="s">
         <v>83</v>
@@ -971,16 +983,16 @@
         <v>91</v>
       </c>
       <c r="G7" t="s">
-        <v>82</v>
-      </c>
-      <c r="H7" t="s">
-        <v>82</v>
+        <v>85</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>118</v>
       </c>
       <c r="J7" t="s">
         <v>83</v>
       </c>
       <c r="K7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -994,7 +1006,7 @@
         <v>13</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G8" t="s">
         <v>82</v>
@@ -1072,7 +1084,7 @@
         <v>13</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G11" t="s">
         <v>82</v>
@@ -1098,7 +1110,7 @@
         <v>13</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G12" t="s">
         <v>82</v>
@@ -1124,7 +1136,7 @@
         <v>13</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G13" t="s">
         <v>82</v>
@@ -1150,7 +1162,7 @@
         <v>13</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G14" t="s">
         <v>82</v>
@@ -1280,7 +1292,7 @@
         <v>13</v>
       </c>
       <c r="F19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G19" t="s">
         <v>82</v>
@@ -1306,7 +1318,7 @@
         <v>13</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G20" t="s">
         <v>82</v>
@@ -1332,7 +1344,7 @@
         <v>13</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G21" t="s">
         <v>82</v>
@@ -1358,7 +1370,7 @@
         <v>13</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G22" t="s">
         <v>82</v>
@@ -1384,7 +1396,7 @@
         <v>13</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G23" t="s">
         <v>82</v>
@@ -1410,7 +1422,7 @@
         <v>13</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G24" t="s">
         <v>82</v>
@@ -1436,7 +1448,7 @@
         <v>13</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G25" t="s">
         <v>82</v>
@@ -1462,7 +1474,7 @@
         <v>13</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G26" t="s">
         <v>82</v>
@@ -1488,7 +1500,7 @@
         <v>13</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G27" t="s">
         <v>82</v>
@@ -1514,13 +1526,13 @@
         <v>13</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G28" t="s">
         <v>85</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J28" t="s">
         <v>83</v>
@@ -1592,7 +1604,7 @@
         <v>13</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G31" t="s">
         <v>82</v>
@@ -1618,7 +1630,7 @@
         <v>13</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G32" t="s">
         <v>82</v>
@@ -1696,19 +1708,19 @@
         <v>13</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G35" t="s">
-        <v>82</v>
-      </c>
-      <c r="H35" t="s">
-        <v>82</v>
+        <v>85</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>121</v>
       </c>
       <c r="J35" t="s">
         <v>83</v>
       </c>
       <c r="K35" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.25">
@@ -1722,13 +1734,13 @@
         <v>13</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G36" t="s">
         <v>85</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J36" t="s">
         <v>83</v>

</xml_diff>